<commit_message>
Update: Error handling + Validation
</commit_message>
<xml_diff>
--- a/output/sample1_extracted.xlsx
+++ b/output/sample1_extracted.xlsx
@@ -505,7 +505,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,11 +534,6 @@
           <t>Transaction Type</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Balance</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -561,9 +556,70 @@
           <t>Debit</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>₹1,10,000.00</t>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>03-05-2024</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ATM Withdrawal</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>5,000.00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Dr</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>05/05/2024</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Salary Credit</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>50,000.00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Credit</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>10-05-2024</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Online Shopping</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2,000.00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Debit</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update: Add additional prompts for documents
</commit_message>
<xml_diff>
--- a/output/sample1_extracted.xlsx
+++ b/output/sample1_extracted.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,6 +462,11 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Branch</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Closing Balance</t>
         </is>
       </c>
@@ -484,15 +489,20 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>01-May-2024 to 31-May-2024</t>
+          <t>01/05/2024 to 31/05/2024</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>₹1,25,000.00</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
+          <t>1,25,000.00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>MG Road, Bangalore</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -505,7 +515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,11 +544,16 @@
           <t>Transaction Type</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Balance</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>02-May-2024</t>
+          <t>02/05/2024</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -548,19 +563,24 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>₹15,000.00</t>
+          <t>15,000.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>Debit</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1,10,000.00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>03-05-2024</t>
+          <t>03/05/2024</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -576,6 +596,11 @@
       <c r="D3" t="inlineStr">
         <is>
           <t>Dr</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>45,000.00</t>
         </is>
       </c>
     </row>
@@ -600,11 +625,16 @@
           <t>Credit</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2,50,000.00</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>10-05-2024</t>
+          <t>10/05/2024</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -620,6 +650,11 @@
       <c r="D5" t="inlineStr">
         <is>
           <t>Debit</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>73,000.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update: Add test files
</commit_message>
<xml_diff>
--- a/output/sample1_extracted.xlsx
+++ b/output/sample1_extracted.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,72 +437,104 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Account Holder Name</t>
+          <t>Bank Name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Branch Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Customer Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Account Number</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Customer ID</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Account Type</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>IFSC Code</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Opening Balance</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Closing Balance</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Period</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Opening Balance</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Branch</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Closing Balance</t>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Generated On</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Bank of Tomorrow Ltd.</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MG Road, Bangalore</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Mr. Rajiv Sharma</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>987654321012</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
         <is>
           <t>BOTM0001234</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>01/05/2024 to 31/05/2024</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1,25,000.00</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>MG Road, Bangalore</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>₹1,25,000.00</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>73,000.00</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>01-May-2024 to 31-May-2024</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -515,7 +547,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,16 +576,11 @@
           <t>Transaction Type</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Balance</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>02/05/2024</t>
+          <t>02-May-2024</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -563,24 +590,19 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>15,000.00</t>
+          <t>₹15,000.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>Debit</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1,10,000.00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>03/05/2024</t>
+          <t>03-05-2024</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -596,11 +618,6 @@
       <c r="D3" t="inlineStr">
         <is>
           <t>Dr</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>45,000.00</t>
         </is>
       </c>
     </row>
@@ -625,16 +642,11 @@
           <t>Credit</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2,50,000.00</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>10/05/2024</t>
+          <t>10-05-2024</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -650,11 +662,6 @@
       <c r="D5" t="inlineStr">
         <is>
           <t>Debit</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>73,000.00</t>
         </is>
       </c>
     </row>

</xml_diff>